<commit_message>
PSPLIB to Excel conversion
</commit_message>
<xml_diff>
--- a/RCPSPPSinputTemplate.xlsx
+++ b/RCPSPPSinputTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16665" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16665" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
@@ -225,7 +225,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>Inputdaten für das RCPSP-PS-Q</t>
   </si>
@@ -394,6 +394,9 @@
   <si>
     <t>c</t>
   </si>
+  <si>
+    <t>kn(j,1)</t>
+  </si>
 </sst>
 </file>
 
@@ -445,7 +448,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -759,11 +762,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -776,9 +875,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -803,9 +899,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,9 +915,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -835,14 +925,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -855,8 +949,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -874,12 +971,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1218,7 +1321,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>597795</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
@@ -1269,7 +1372,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>597795</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
@@ -1320,7 +1423,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>597795</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
@@ -1371,7 +1474,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>597795</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
@@ -1422,7 +1525,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>597795</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
@@ -2080,7 +2183,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2384,38 +2487,38 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2448,9 +2551,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2692,39 +2793,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
@@ -2764,7 +2865,7 @@
         <v>1</v>
       </c>
       <c r="S5" t="str">
-        <f>Demo!D6</f>
+        <f>Demo!E6</f>
         <v>yes</v>
       </c>
       <c r="U5">
@@ -2788,7 +2889,7 @@
         <v>2</v>
       </c>
       <c r="S6" t="str">
-        <f>Demo!D7</f>
+        <f>Demo!E7</f>
         <v>yes</v>
       </c>
     </row>
@@ -2804,7 +2905,7 @@
         <v>3</v>
       </c>
       <c r="S7" t="str">
-        <f>Demo!D8</f>
+        <f>Demo!E8</f>
         <v>yes</v>
       </c>
     </row>
@@ -2820,7 +2921,7 @@
         <v>4</v>
       </c>
       <c r="S8">
-        <f>Demo!D9</f>
+        <f>Demo!E9</f>
         <v>0</v>
       </c>
     </row>
@@ -2836,7 +2937,7 @@
         <v>5</v>
       </c>
       <c r="S9">
-        <f>Demo!D10</f>
+        <f>Demo!E10</f>
         <v>0</v>
       </c>
     </row>
@@ -2852,7 +2953,7 @@
         <v>6</v>
       </c>
       <c r="S10" t="str">
-        <f>Demo!D11</f>
+        <f>Demo!E11</f>
         <v>yes</v>
       </c>
     </row>
@@ -2868,7 +2969,7 @@
         <v>7</v>
       </c>
       <c r="S11">
-        <f>Demo!D12</f>
+        <f>Demo!E12</f>
         <v>0</v>
       </c>
     </row>
@@ -2884,7 +2985,7 @@
         <v>8</v>
       </c>
       <c r="S12">
-        <f>Demo!D13</f>
+        <f>Demo!E13</f>
         <v>0</v>
       </c>
     </row>
@@ -2900,7 +3001,7 @@
         <v>9</v>
       </c>
       <c r="S13">
-        <f>Demo!D14</f>
+        <f>Demo!E14</f>
         <v>0</v>
       </c>
     </row>
@@ -2916,7 +3017,7 @@
         <v>10</v>
       </c>
       <c r="S14" t="str">
-        <f>Demo!D15</f>
+        <f>Demo!E15</f>
         <v>yes</v>
       </c>
     </row>
@@ -2937,38 +3038,38 @@
   <dimension ref="A1:BZ28"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="BW7" sqref="BW7"/>
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:78" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="R1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
+      <c r="R1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
     </row>
     <row r="2" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="R2" s="38" t="s">
+      <c r="R2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
     </row>
     <row r="5" spans="1:78" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2977,9 +3078,6 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
@@ -3067,94 +3165,90 @@
         <f>Demo!G6</f>
         <v>yes</v>
       </c>
-      <c r="C6">
-        <f>Demo!H6</f>
-        <v>0</v>
-      </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
+        <f>Demo!H6</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
         <f>Demo!I6</f>
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f>Demo!J6</f>
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f>Demo!K6</f>
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f>Demo!L6</f>
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f>Demo!M6</f>
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f>Demo!N6</f>
         <v>0</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f>Demo!O6</f>
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f>Demo!P6</f>
         <v>0</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <f>Demo!Q6</f>
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <f>Demo!R6</f>
         <v>0</v>
       </c>
       <c r="T6">
         <v>1</v>
       </c>
       <c r="U6">
-        <f>Demo!$E6</f>
+        <f>Demo!$F6</f>
         <v>0</v>
       </c>
       <c r="V6">
-        <f>Demo!$E7</f>
+        <f>Demo!$F7</f>
         <v>0</v>
       </c>
       <c r="W6">
-        <f>Demo!$E8</f>
+        <f>Demo!$F8</f>
         <v>0</v>
       </c>
       <c r="X6" t="str">
-        <f>Demo!$E9</f>
+        <f>Demo!$F9</f>
         <v>yes</v>
       </c>
       <c r="Y6" t="str">
-        <f>Demo!$E10</f>
+        <f>Demo!$F10</f>
         <v>yes</v>
       </c>
       <c r="Z6">
-        <f>Demo!$E11</f>
+        <f>Demo!$F11</f>
         <v>0</v>
       </c>
       <c r="AA6">
-        <f>Demo!$E12</f>
+        <f>Demo!$F12</f>
         <v>0</v>
       </c>
       <c r="AB6">
-        <f>Demo!$E13</f>
+        <f>Demo!$F13</f>
         <v>0</v>
       </c>
       <c r="AC6">
-        <f>Demo!$E14</f>
+        <f>Demo!$F14</f>
         <v>0</v>
       </c>
       <c r="AD6">
-        <f>Demo!$E15</f>
+        <f>Demo!$F15</f>
         <v>0</v>
       </c>
       <c r="BV6">
@@ -3168,6 +3262,7 @@
         <v>1</v>
       </c>
       <c r="BZ6">
+        <f>Demo!D6</f>
         <v>0</v>
       </c>
     </row>
@@ -3179,94 +3274,47 @@
         <f>Demo!G7</f>
         <v>0</v>
       </c>
-      <c r="C7">
-        <f>Demo!H7</f>
-        <v>0</v>
-      </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7">
+        <f>Demo!H7</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
         <f>Demo!I7</f>
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f>Demo!J7</f>
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f>Demo!K7</f>
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f>Demo!L7</f>
         <v>0</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f>Demo!M7</f>
         <v>0</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f>Demo!N7</f>
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f>Demo!O7</f>
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f>Demo!P7</f>
         <v>0</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <f>Demo!Q7</f>
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <f>Demo!R7</f>
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>2</v>
-      </c>
-      <c r="U7">
-        <f>Demo!F6</f>
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <f>Demo!$F7</f>
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <f>Demo!$F8</f>
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <f>Demo!$F9</f>
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <f>Demo!$F10</f>
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <f>Demo!$F11</f>
-        <v>0</v>
-      </c>
-      <c r="AA7" t="str">
-        <f>Demo!$F12</f>
-        <v>yes</v>
-      </c>
-      <c r="AB7" t="str">
-        <f>Demo!$F13</f>
-        <v>yes</v>
-      </c>
-      <c r="AC7">
-        <f>Demo!$F14</f>
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <f>Demo!$F15</f>
         <v>0</v>
       </c>
       <c r="BV7">
@@ -3280,6 +3328,7 @@
         <v>2</v>
       </c>
       <c r="BZ7">
+        <f>Demo!D7</f>
         <v>0</v>
       </c>
     </row>
@@ -3291,51 +3340,47 @@
         <f>Demo!G8</f>
         <v>0</v>
       </c>
-      <c r="C8">
-        <f>Demo!H8</f>
-        <v>0</v>
-      </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8">
+        <f>Demo!H8</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
         <f>Demo!I8</f>
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f>Demo!J8</f>
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f>Demo!K8</f>
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f>Demo!L8</f>
         <v>0</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f>Demo!M8</f>
         <v>0</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f>Demo!N8</f>
         <v>0</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f>Demo!O8</f>
         <v>0</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f>Demo!P8</f>
         <v>0</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <f>Demo!Q8</f>
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <f>Demo!R8</f>
         <v>0</v>
       </c>
       <c r="BV8">
@@ -3349,6 +3394,7 @@
         <v>3</v>
       </c>
       <c r="BZ8">
+        <f>Demo!D8</f>
         <v>0</v>
       </c>
     </row>
@@ -3360,51 +3406,47 @@
         <f>Demo!G9</f>
         <v>0</v>
       </c>
-      <c r="C9">
-        <f>Demo!H9</f>
-        <v>0</v>
-      </c>
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9">
+        <f>Demo!H9</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
         <f>Demo!I9</f>
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f>Demo!J9</f>
         <v>0</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f>Demo!K9</f>
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f>Demo!L9</f>
         <v>0</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f>Demo!M9</f>
         <v>0</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f>Demo!N9</f>
         <v>0</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f>Demo!O9</f>
         <v>0</v>
       </c>
-      <c r="M9">
+      <c r="N9" t="str">
         <f>Demo!P9</f>
-        <v>0</v>
-      </c>
-      <c r="N9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="O9">
         <f>Demo!Q9</f>
-        <v>yes</v>
-      </c>
-      <c r="O9">
-        <f>Demo!R9</f>
         <v>0</v>
       </c>
       <c r="BV9">
@@ -3418,6 +3460,7 @@
         <v>4</v>
       </c>
       <c r="BZ9">
+        <f>Demo!D9</f>
         <v>0</v>
       </c>
     </row>
@@ -3429,51 +3472,47 @@
         <f>Demo!G10</f>
         <v>0</v>
       </c>
-      <c r="C10" t="str">
-        <f>Demo!H10</f>
-        <v>yes</v>
-      </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
+        <f>Demo!H10</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
         <f>Demo!I10</f>
         <v>0</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f>Demo!J10</f>
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f>Demo!K10</f>
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f>Demo!L10</f>
         <v>0</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f>Demo!M10</f>
         <v>0</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <f>Demo!N10</f>
         <v>0</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f>Demo!O10</f>
         <v>0</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <f>Demo!P10</f>
         <v>0</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <f>Demo!Q10</f>
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <f>Demo!R10</f>
         <v>0</v>
       </c>
       <c r="BV10">
@@ -3487,6 +3526,7 @@
         <v>5</v>
       </c>
       <c r="BZ10">
+        <f>Demo!D10</f>
         <v>0</v>
       </c>
     </row>
@@ -3498,51 +3538,47 @@
         <f>Demo!G11</f>
         <v>0</v>
       </c>
-      <c r="C11">
-        <f>Demo!H11</f>
-        <v>0</v>
-      </c>
       <c r="E11">
         <v>6</v>
       </c>
       <c r="F11">
+        <f>Demo!H11</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
         <f>Demo!I11</f>
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f>Demo!J11</f>
         <v>0</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f>Demo!K11</f>
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f>Demo!L11</f>
         <v>0</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f>Demo!M11</f>
         <v>0</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <f>Demo!N11</f>
         <v>0</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f>Demo!O11</f>
         <v>0</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <f>Demo!P11</f>
         <v>0</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <f>Demo!Q11</f>
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <f>Demo!R11</f>
         <v>0</v>
       </c>
       <c r="BV11">
@@ -3556,6 +3592,7 @@
         <v>6</v>
       </c>
       <c r="BZ11">
+        <f>Demo!D11</f>
         <v>0</v>
       </c>
     </row>
@@ -3567,51 +3604,47 @@
         <f>Demo!G12</f>
         <v>0</v>
       </c>
-      <c r="C12">
-        <f>Demo!H12</f>
-        <v>0</v>
-      </c>
       <c r="E12">
         <v>7</v>
       </c>
       <c r="F12">
+        <f>Demo!H12</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
         <f>Demo!I12</f>
         <v>0</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f>Demo!J12</f>
         <v>0</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f>Demo!K12</f>
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f>Demo!L12</f>
         <v>0</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f>Demo!M12</f>
         <v>0</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <f>Demo!N12</f>
         <v>0</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f>Demo!O12</f>
         <v>0</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f>Demo!P12</f>
         <v>0</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <f>Demo!Q12</f>
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <f>Demo!R12</f>
         <v>0</v>
       </c>
       <c r="BV12">
@@ -3625,6 +3658,7 @@
         <v>7</v>
       </c>
       <c r="BZ12">
+        <f>Demo!D12</f>
         <v>0</v>
       </c>
     </row>
@@ -3636,51 +3670,47 @@
         <f>Demo!G13</f>
         <v>0</v>
       </c>
-      <c r="C13">
-        <f>Demo!H13</f>
-        <v>0</v>
-      </c>
       <c r="E13">
         <v>8</v>
       </c>
       <c r="F13">
+        <f>Demo!H13</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
         <f>Demo!I13</f>
         <v>0</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f>Demo!J13</f>
         <v>0</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f>Demo!K13</f>
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f>Demo!L13</f>
         <v>0</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f>Demo!M13</f>
         <v>0</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <f>Demo!N13</f>
         <v>0</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f>Demo!O13</f>
         <v>0</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <f>Demo!P13</f>
         <v>0</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <f>Demo!Q13</f>
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <f>Demo!R13</f>
         <v>0</v>
       </c>
       <c r="BV13">
@@ -3694,6 +3724,7 @@
         <v>8</v>
       </c>
       <c r="BZ13">
+        <f>Demo!D13</f>
         <v>0</v>
       </c>
     </row>
@@ -3705,51 +3736,47 @@
         <f>Demo!G14</f>
         <v>0</v>
       </c>
-      <c r="C14">
-        <f>Demo!H14</f>
-        <v>0</v>
-      </c>
       <c r="E14">
         <v>9</v>
       </c>
       <c r="F14">
+        <f>Demo!H14</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
         <f>Demo!I14</f>
         <v>0</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f>Demo!J14</f>
         <v>0</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f>Demo!K14</f>
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f>Demo!L14</f>
         <v>0</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f>Demo!M14</f>
         <v>0</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <f>Demo!N14</f>
         <v>0</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f>Demo!O14</f>
         <v>0</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <f>Demo!P14</f>
         <v>0</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <f>Demo!Q14</f>
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <f>Demo!R14</f>
         <v>0</v>
       </c>
       <c r="BV14">
@@ -3763,6 +3790,7 @@
         <v>9</v>
       </c>
       <c r="BZ14">
+        <f>Demo!D14</f>
         <v>0</v>
       </c>
     </row>
@@ -3774,51 +3802,47 @@
         <f>Demo!G15</f>
         <v>0</v>
       </c>
-      <c r="C15">
-        <f>Demo!H15</f>
-        <v>0</v>
-      </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15">
+        <f>Demo!H15</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
         <f>Demo!I15</f>
         <v>0</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f>Demo!J15</f>
         <v>0</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f>Demo!K15</f>
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f>Demo!L15</f>
         <v>0</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f>Demo!M15</f>
         <v>0</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <f>Demo!N15</f>
         <v>0</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f>Demo!O15</f>
         <v>0</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <f>Demo!P15</f>
         <v>0</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <f>Demo!Q15</f>
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <f>Demo!R15</f>
         <v>0</v>
       </c>
       <c r="BV15">
@@ -3832,6 +3856,7 @@
         <v>10</v>
       </c>
       <c r="BZ15">
+        <f>Demo!D15</f>
         <v>0</v>
       </c>
     </row>
@@ -3875,43 +3900,43 @@
         <v>1</v>
       </c>
       <c r="F19">
+        <f>Demo!R6</f>
+        <v>0</v>
+      </c>
+      <c r="G19" t="str">
         <f>Demo!S6</f>
-        <v>0</v>
-      </c>
-      <c r="G19" t="str">
+        <v>yes</v>
+      </c>
+      <c r="H19" t="str">
         <f>Demo!T6</f>
         <v>yes</v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19">
         <f>Demo!U6</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>Demo!V6</f>
+        <v>0</v>
+      </c>
+      <c r="K19" t="str">
+        <f>Demo!W6</f>
         <v>yes</v>
       </c>
-      <c r="I19">
-        <f>Demo!V6</f>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <f>Demo!W6</f>
-        <v>0</v>
-      </c>
-      <c r="K19" t="str">
+      <c r="L19">
         <f>Demo!X6</f>
-        <v>yes</v>
-      </c>
-      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
         <f>Demo!Y6</f>
         <v>0</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <f>Demo!Z6</f>
         <v>0</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <f>Demo!AA6</f>
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <f>Demo!AB6</f>
         <v>0</v>
       </c>
     </row>
@@ -3920,43 +3945,43 @@
         <v>2</v>
       </c>
       <c r="F20">
+        <f>Demo!R7</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
         <f>Demo!S7</f>
         <v>0</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f>Demo!T7</f>
         <v>0</v>
       </c>
-      <c r="H20">
+      <c r="I20" t="str">
         <f>Demo!U7</f>
-        <v>0</v>
-      </c>
-      <c r="I20" t="str">
+        <v>yes</v>
+      </c>
+      <c r="J20" t="str">
         <f>Demo!V7</f>
         <v>yes</v>
       </c>
-      <c r="J20" t="str">
+      <c r="K20">
         <f>Demo!W7</f>
-        <v>yes</v>
-      </c>
-      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
         <f>Demo!X7</f>
         <v>0</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f>Demo!Y7</f>
         <v>0</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <f>Demo!Z7</f>
         <v>0</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <f>Demo!AA7</f>
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <f>Demo!AB7</f>
         <v>0</v>
       </c>
     </row>
@@ -3965,43 +3990,43 @@
         <v>3</v>
       </c>
       <c r="F21">
+        <f>Demo!R8</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
         <f>Demo!S8</f>
         <v>0</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f>Demo!T8</f>
         <v>0</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <f>Demo!U8</f>
         <v>0</v>
       </c>
-      <c r="I21">
+      <c r="J21" t="str">
         <f>Demo!V8</f>
-        <v>0</v>
-      </c>
-      <c r="J21" t="str">
+        <v>yes</v>
+      </c>
+      <c r="K21">
         <f>Demo!W8</f>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f>Demo!X8</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>Demo!Y8</f>
+        <v>0</v>
+      </c>
+      <c r="N21" t="str">
+        <f>Demo!Z8</f>
         <v>yes</v>
       </c>
-      <c r="K21">
-        <f>Demo!X8</f>
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <f>Demo!Y8</f>
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <f>Demo!Z8</f>
-        <v>0</v>
-      </c>
-      <c r="N21" t="str">
+      <c r="O21">
         <f>Demo!AA8</f>
-        <v>yes</v>
-      </c>
-      <c r="O21">
-        <f>Demo!AB8</f>
         <v>0</v>
       </c>
     </row>
@@ -4010,43 +4035,43 @@
         <v>4</v>
       </c>
       <c r="F22">
+        <f>Demo!R9</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
         <f>Demo!S9</f>
         <v>0</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f>Demo!T9</f>
         <v>0</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <f>Demo!U9</f>
         <v>0</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <f>Demo!V9</f>
         <v>0</v>
       </c>
-      <c r="J22">
+      <c r="K22" t="str">
         <f>Demo!W9</f>
-        <v>0</v>
-      </c>
-      <c r="K22" t="str">
+        <v>yes</v>
+      </c>
+      <c r="L22">
         <f>Demo!X9</f>
-        <v>yes</v>
-      </c>
-      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
         <f>Demo!Y9</f>
         <v>0</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <f>Demo!Z9</f>
         <v>0</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <f>Demo!AA9</f>
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <f>Demo!AB9</f>
         <v>0</v>
       </c>
     </row>
@@ -4055,43 +4080,43 @@
         <v>5</v>
       </c>
       <c r="F23">
+        <f>Demo!R10</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
         <f>Demo!S10</f>
         <v>0</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f>Demo!T10</f>
         <v>0</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f>Demo!U10</f>
         <v>0</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f>Demo!V10</f>
         <v>0</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f>Demo!W10</f>
         <v>0</v>
       </c>
-      <c r="K23">
+      <c r="L23" t="str">
         <f>Demo!X10</f>
-        <v>0</v>
-      </c>
-      <c r="L23" t="str">
+        <v>yes</v>
+      </c>
+      <c r="M23" t="str">
         <f>Demo!Y10</f>
         <v>yes</v>
       </c>
-      <c r="M23" t="str">
+      <c r="N23">
         <f>Demo!Z10</f>
-        <v>yes</v>
-      </c>
-      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
         <f>Demo!AA10</f>
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <f>Demo!AB10</f>
         <v>0</v>
       </c>
     </row>
@@ -4100,43 +4125,43 @@
         <v>6</v>
       </c>
       <c r="F24">
+        <f>Demo!R11</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
         <f>Demo!S11</f>
         <v>0</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f>Demo!T11</f>
         <v>0</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <f>Demo!U11</f>
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f>Demo!V11</f>
         <v>0</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f>Demo!W11</f>
         <v>0</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <f>Demo!X11</f>
         <v>0</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <f>Demo!Y11</f>
         <v>0</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <f>Demo!Z11</f>
         <v>0</v>
       </c>
-      <c r="N24">
+      <c r="O24" t="str">
         <f>Demo!AA11</f>
-        <v>0</v>
-      </c>
-      <c r="O24" t="str">
-        <f>Demo!AB11</f>
         <v>yes</v>
       </c>
     </row>
@@ -4145,43 +4170,43 @@
         <v>7</v>
       </c>
       <c r="F25">
+        <f>Demo!R12</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
         <f>Demo!S12</f>
         <v>0</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f>Demo!T12</f>
         <v>0</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <f>Demo!U12</f>
         <v>0</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f>Demo!V12</f>
         <v>0</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <f>Demo!W12</f>
         <v>0</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <f>Demo!X12</f>
         <v>0</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <f>Demo!Y12</f>
         <v>0</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <f>Demo!Z12</f>
         <v>0</v>
       </c>
-      <c r="N25">
+      <c r="O25" t="str">
         <f>Demo!AA12</f>
-        <v>0</v>
-      </c>
-      <c r="O25" t="str">
-        <f>Demo!AB12</f>
         <v>yes</v>
       </c>
     </row>
@@ -4190,43 +4215,43 @@
         <v>8</v>
       </c>
       <c r="F26">
+        <f>Demo!R13</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
         <f>Demo!S13</f>
         <v>0</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f>Demo!T13</f>
         <v>0</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <f>Demo!U13</f>
         <v>0</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f>Demo!V13</f>
         <v>0</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <f>Demo!W13</f>
         <v>0</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <f>Demo!X13</f>
         <v>0</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <f>Demo!Y13</f>
         <v>0</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <f>Demo!Z13</f>
         <v>0</v>
       </c>
-      <c r="N26">
+      <c r="O26" t="str">
         <f>Demo!AA13</f>
-        <v>0</v>
-      </c>
-      <c r="O26" t="str">
-        <f>Demo!AB13</f>
         <v>yes</v>
       </c>
     </row>
@@ -4235,43 +4260,43 @@
         <v>9</v>
       </c>
       <c r="F27">
+        <f>Demo!R14</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
         <f>Demo!S14</f>
         <v>0</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f>Demo!T14</f>
         <v>0</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <f>Demo!U14</f>
         <v>0</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f>Demo!V14</f>
         <v>0</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <f>Demo!W14</f>
         <v>0</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <f>Demo!X14</f>
         <v>0</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <f>Demo!Y14</f>
         <v>0</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <f>Demo!Z14</f>
         <v>0</v>
       </c>
-      <c r="N27">
+      <c r="O27" t="str">
         <f>Demo!AA14</f>
-        <v>0</v>
-      </c>
-      <c r="O27" t="str">
-        <f>Demo!AB14</f>
         <v>yes</v>
       </c>
     </row>
@@ -4280,43 +4305,43 @@
         <v>10</v>
       </c>
       <c r="F28">
+        <f>Demo!R15</f>
+        <v>0</v>
+      </c>
+      <c r="G28">
         <f>Demo!S15</f>
         <v>0</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f>Demo!T15</f>
         <v>0</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <f>Demo!U15</f>
         <v>0</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f>Demo!V15</f>
         <v>0</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <f>Demo!W15</f>
         <v>0</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <f>Demo!X15</f>
         <v>0</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <f>Demo!Y15</f>
         <v>0</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <f>Demo!Z15</f>
         <v>0</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <f>Demo!AA15</f>
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <f>Demo!AB15</f>
         <v>0</v>
       </c>
     </row>
@@ -4344,19 +4369,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="F3" s="40" t="s">
+      <c r="B3" s="40"/>
+      <c r="F3" s="41" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4370,7 +4395,7 @@
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="40"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -4458,47 +4483,46 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-    </row>
-    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4506,618 +4530,617 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48" t="s">
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="49" t="s">
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49"/>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-    </row>
-    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="43"/>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="F4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42" t="s">
+      <c r="H4" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="43" t="s">
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-    </row>
-    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="5">
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="45"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="5">
         <v>1</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2</v>
       </c>
       <c r="G5" s="5">
         <v>1</v>
       </c>
       <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
         <v>2</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
+        <v>3</v>
+      </c>
+      <c r="K5" s="7">
+        <v>4</v>
+      </c>
+      <c r="L5" s="7">
+        <v>5</v>
+      </c>
+      <c r="M5" s="7">
+        <v>6</v>
+      </c>
+      <c r="N5" s="7">
+        <v>7</v>
+      </c>
+      <c r="O5" s="7">
+        <v>8</v>
+      </c>
+      <c r="P5" s="7">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>10</v>
+      </c>
+      <c r="R5" s="9">
         <v>1</v>
       </c>
-      <c r="J5" s="8">
+      <c r="S5" s="10">
         <v>2</v>
       </c>
-      <c r="K5" s="8">
+      <c r="T5" s="10">
         <v>3</v>
       </c>
-      <c r="L5" s="8">
+      <c r="U5" s="10">
         <v>4</v>
       </c>
-      <c r="M5" s="8">
+      <c r="V5" s="10">
         <v>5</v>
       </c>
-      <c r="N5" s="8">
+      <c r="W5" s="10">
         <v>6</v>
       </c>
-      <c r="O5" s="8">
+      <c r="X5" s="10">
         <v>7</v>
       </c>
-      <c r="P5" s="8">
+      <c r="Y5" s="10">
         <v>8</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Z5" s="10">
         <v>9</v>
       </c>
-      <c r="R5" s="9">
+      <c r="AA5" s="11">
         <v>10</v>
       </c>
-      <c r="S5" s="10">
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
         <v>1</v>
       </c>
-      <c r="T5" s="11">
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="34">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="15"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="U5" s="11">
+      <c r="B7" s="21">
         <v>3</v>
       </c>
-      <c r="V5" s="11">
+      <c r="C7" s="23">
+        <v>3</v>
+      </c>
+      <c r="D7" s="35">
+        <v>0</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="23"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>3</v>
+      </c>
+      <c r="B8" s="21">
         <v>4</v>
       </c>
-      <c r="W5" s="11">
+      <c r="C8" s="23">
+        <v>7</v>
+      </c>
+      <c r="D8" s="35">
+        <v>0</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="23"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <v>4</v>
+      </c>
+      <c r="B9" s="21">
+        <v>3</v>
+      </c>
+      <c r="C9" s="23">
         <v>5</v>
       </c>
-      <c r="X5" s="11">
+      <c r="D9" s="35">
+        <v>0</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="23"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
+        <v>5</v>
+      </c>
+      <c r="B10" s="21">
+        <v>5</v>
+      </c>
+      <c r="C10" s="23">
+        <v>2</v>
+      </c>
+      <c r="D10" s="35">
+        <v>0</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="23"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
         <v>6</v>
       </c>
-      <c r="Y5" s="11">
+      <c r="B11" s="21">
+        <v>6</v>
+      </c>
+      <c r="C11" s="23">
+        <v>8</v>
+      </c>
+      <c r="D11" s="35">
+        <v>0</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
         <v>7</v>
       </c>
-      <c r="Z5" s="11">
+      <c r="B12" s="21">
+        <v>4</v>
+      </c>
+      <c r="C12" s="23">
+        <v>6</v>
+      </c>
+      <c r="D12" s="35">
+        <v>0</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="22"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
+      <c r="AA12" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
         <v>8</v>
       </c>
-      <c r="AA5" s="11">
+      <c r="B13" s="21">
+        <v>2</v>
+      </c>
+      <c r="C13" s="23">
+        <v>5</v>
+      </c>
+      <c r="D13" s="35">
+        <v>0</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="22"/>
+      <c r="AA13" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
         <v>9</v>
       </c>
-      <c r="AB5" s="12">
+      <c r="B14" s="21">
+        <v>2</v>
+      </c>
+      <c r="C14" s="23">
+        <v>4</v>
+      </c>
+      <c r="D14" s="35">
+        <v>0</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
+      <c r="AA14" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>1</v>
-      </c>
-      <c r="B6" s="14">
-        <v>0</v>
-      </c>
-      <c r="C6" s="16">
-        <v>0</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="36">
+        <v>0</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="16"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
-        <v>2</v>
-      </c>
-      <c r="B7" s="23">
-        <v>3</v>
-      </c>
-      <c r="C7" s="25">
-        <v>3</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="W7" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="24"/>
-      <c r="AB7" s="25"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
-        <v>3</v>
-      </c>
-      <c r="B8" s="23">
-        <v>4</v>
-      </c>
-      <c r="C8" s="25">
-        <v>7</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB8" s="25"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>4</v>
-      </c>
-      <c r="B9" s="23">
-        <v>3</v>
-      </c>
-      <c r="C9" s="25">
-        <v>5</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="R9" s="30"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="24"/>
-      <c r="AB9" s="25"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
-        <v>5</v>
-      </c>
-      <c r="B10" s="23">
-        <v>5</v>
-      </c>
-      <c r="C10" s="25">
-        <v>2</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z10" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="25"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
-        <v>6</v>
-      </c>
-      <c r="B11" s="23">
-        <v>6</v>
-      </c>
-      <c r="C11" s="25">
-        <v>8</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="24"/>
-      <c r="AB11" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
-        <v>7</v>
-      </c>
-      <c r="B12" s="23">
-        <v>4</v>
-      </c>
-      <c r="C12" s="25">
-        <v>6</v>
-      </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
-        <v>8</v>
-      </c>
-      <c r="B13" s="23">
-        <v>2</v>
-      </c>
-      <c r="C13" s="25">
-        <v>5</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="24"/>
-      <c r="U13" s="24"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24"/>
-      <c r="AA13" s="24"/>
-      <c r="AB13" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
-        <v>9</v>
-      </c>
-      <c r="B14" s="23">
-        <v>2</v>
-      </c>
-      <c r="C14" s="25">
-        <v>4</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31">
-        <v>10</v>
-      </c>
-      <c r="B15" s="10">
-        <v>0</v>
-      </c>
-      <c r="C15" s="12">
-        <v>0</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="33"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
       <c r="AA15" s="11"/>
-      <c r="AB15" s="12"/>
-    </row>
-    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+    </row>
+    <row r="16" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="31">
         <f>SUM(B6:B15)</f>
         <v>29</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="31">
         <v>10</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="34"/>
-      <c r="U16" s="34"/>
-      <c r="V16" s="34"/>
-      <c r="W16" s="34"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="34"/>
-      <c r="Z16" s="34"/>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="34"/>
+      <c r="D16" s="37">
+        <v>10</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="30"/>
+      <c r="AA16" s="30"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5136,19 +5159,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A1:AB1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:R3"/>
-    <mergeCell ref="S3:AB3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:R4"/>
-    <mergeCell ref="S4:AB4"/>
+  <mergeCells count="11">
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="E3:Q3"/>
+    <mergeCell ref="R3:AA3"/>
+    <mergeCell ref="H4:Q4"/>
+    <mergeCell ref="R4:AA4"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>